<commit_message>
added more data and figures
</commit_message>
<xml_diff>
--- a/data/final_transformed_data.xlsx
+++ b/data/final_transformed_data.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>frequency_count</t>
+          <t>frequency</t>
         </is>
       </c>
     </row>
@@ -16541,7 +16541,9 @@
       <c r="A1283" t="n">
         <v>1282</v>
       </c>
-      <c r="B1283" t="inlineStr"/>
+      <c r="B1283" t="n">
+        <v>93</v>
+      </c>
       <c r="C1283" t="n">
         <v>1</v>
       </c>
@@ -16553,7 +16555,9 @@
       <c r="A1284" t="n">
         <v>1283</v>
       </c>
-      <c r="B1284" t="inlineStr"/>
+      <c r="B1284" t="n">
+        <v>93</v>
+      </c>
       <c r="C1284" t="n">
         <v>6</v>
       </c>
@@ -16563,7 +16567,9 @@
       <c r="A1285" t="n">
         <v>1284</v>
       </c>
-      <c r="B1285" t="inlineStr"/>
+      <c r="B1285" t="n">
+        <v>93</v>
+      </c>
       <c r="C1285" t="n">
         <v>3</v>
       </c>
@@ -16575,7 +16581,9 @@
       <c r="A1286" t="n">
         <v>1285</v>
       </c>
-      <c r="B1286" t="inlineStr"/>
+      <c r="B1286" t="n">
+        <v>93</v>
+      </c>
       <c r="C1286" t="n">
         <v>4</v>
       </c>
@@ -16587,7 +16595,9 @@
       <c r="A1287" t="n">
         <v>1286</v>
       </c>
-      <c r="B1287" t="inlineStr"/>
+      <c r="B1287" t="n">
+        <v>93</v>
+      </c>
       <c r="C1287" t="n">
         <v>5</v>
       </c>
@@ -16599,7 +16609,9 @@
       <c r="A1288" t="n">
         <v>1287</v>
       </c>
-      <c r="B1288" t="inlineStr"/>
+      <c r="B1288" t="n">
+        <v>93</v>
+      </c>
       <c r="C1288" t="n">
         <v>6</v>
       </c>
@@ -16609,7 +16621,9 @@
       <c r="A1289" t="n">
         <v>1288</v>
       </c>
-      <c r="B1289" t="inlineStr"/>
+      <c r="B1289" t="n">
+        <v>93</v>
+      </c>
       <c r="C1289" t="n">
         <v>7</v>
       </c>
@@ -16621,7 +16635,9 @@
       <c r="A1290" t="n">
         <v>1289</v>
       </c>
-      <c r="B1290" t="inlineStr"/>
+      <c r="B1290" t="n">
+        <v>93</v>
+      </c>
       <c r="C1290" t="n">
         <v>8</v>
       </c>
@@ -16633,7 +16649,9 @@
       <c r="A1291" t="n">
         <v>1290</v>
       </c>
-      <c r="B1291" t="inlineStr"/>
+      <c r="B1291" t="n">
+        <v>93</v>
+      </c>
       <c r="C1291" t="n">
         <v>9</v>
       </c>
@@ -16645,7 +16663,9 @@
       <c r="A1292" t="n">
         <v>1291</v>
       </c>
-      <c r="B1292" t="inlineStr"/>
+      <c r="B1292" t="n">
+        <v>93</v>
+      </c>
       <c r="C1292" t="n">
         <v>10</v>
       </c>
@@ -16655,7 +16675,9 @@
       <c r="A1293" t="n">
         <v>1292</v>
       </c>
-      <c r="B1293" t="inlineStr"/>
+      <c r="B1293" t="n">
+        <v>93</v>
+      </c>
       <c r="C1293" t="n">
         <v>11</v>
       </c>
@@ -16667,7 +16689,9 @@
       <c r="A1294" t="n">
         <v>1293</v>
       </c>
-      <c r="B1294" t="inlineStr"/>
+      <c r="B1294" t="n">
+        <v>93</v>
+      </c>
       <c r="C1294" t="n">
         <v>12</v>
       </c>
@@ -16677,7 +16701,9 @@
       <c r="A1295" t="n">
         <v>1294</v>
       </c>
-      <c r="B1295" t="inlineStr"/>
+      <c r="B1295" t="n">
+        <v>93</v>
+      </c>
       <c r="C1295" t="n">
         <v>13</v>
       </c>
@@ -16689,7 +16715,9 @@
       <c r="A1296" t="n">
         <v>1295</v>
       </c>
-      <c r="B1296" t="inlineStr"/>
+      <c r="B1296" t="n">
+        <v>93</v>
+      </c>
       <c r="C1296" t="n">
         <v>14</v>
       </c>
@@ -16699,7 +16727,9 @@
       <c r="A1297" t="n">
         <v>1296</v>
       </c>
-      <c r="B1297" t="inlineStr"/>
+      <c r="B1297" t="n">
+        <v>93</v>
+      </c>
       <c r="C1297" t="n">
         <v>15</v>
       </c>
@@ -16711,7 +16741,9 @@
       <c r="A1298" t="n">
         <v>1297</v>
       </c>
-      <c r="B1298" t="inlineStr"/>
+      <c r="B1298" t="n">
+        <v>93</v>
+      </c>
       <c r="C1298" t="n">
         <v>16</v>
       </c>
@@ -16721,7 +16753,9 @@
       <c r="A1299" t="n">
         <v>1298</v>
       </c>
-      <c r="B1299" t="inlineStr"/>
+      <c r="B1299" t="n">
+        <v>93</v>
+      </c>
       <c r="C1299" t="n">
         <v>17</v>
       </c>
@@ -16733,7 +16767,9 @@
       <c r="A1300" t="n">
         <v>1299</v>
       </c>
-      <c r="B1300" t="inlineStr"/>
+      <c r="B1300" t="n">
+        <v>93</v>
+      </c>
       <c r="C1300" t="n">
         <v>18</v>
       </c>
@@ -16743,7 +16779,9 @@
       <c r="A1301" t="n">
         <v>1300</v>
       </c>
-      <c r="B1301" t="inlineStr"/>
+      <c r="B1301" t="n">
+        <v>93</v>
+      </c>
       <c r="C1301" t="n">
         <v>19</v>
       </c>
@@ -16755,7 +16793,9 @@
       <c r="A1302" t="n">
         <v>1301</v>
       </c>
-      <c r="B1302" t="inlineStr"/>
+      <c r="B1302" t="n">
+        <v>93</v>
+      </c>
       <c r="C1302" t="n">
         <v>20</v>
       </c>
@@ -16765,7 +16805,9 @@
       <c r="A1303" t="n">
         <v>1302</v>
       </c>
-      <c r="B1303" t="inlineStr"/>
+      <c r="B1303" t="n">
+        <v>93</v>
+      </c>
       <c r="C1303" t="n">
         <v>21</v>
       </c>
@@ -16777,7 +16819,9 @@
       <c r="A1304" t="n">
         <v>1303</v>
       </c>
-      <c r="B1304" t="inlineStr"/>
+      <c r="B1304" t="n">
+        <v>94</v>
+      </c>
       <c r="C1304" t="n">
         <v>1</v>
       </c>
@@ -16787,7 +16831,9 @@
       <c r="A1305" t="n">
         <v>1304</v>
       </c>
-      <c r="B1305" t="inlineStr"/>
+      <c r="B1305" t="n">
+        <v>94</v>
+      </c>
       <c r="C1305" t="n">
         <v>6</v>
       </c>
@@ -16797,7 +16843,9 @@
       <c r="A1306" t="n">
         <v>1305</v>
       </c>
-      <c r="B1306" t="inlineStr"/>
+      <c r="B1306" t="n">
+        <v>94</v>
+      </c>
       <c r="C1306" t="n">
         <v>3</v>
       </c>
@@ -16809,7 +16857,9 @@
       <c r="A1307" t="n">
         <v>1306</v>
       </c>
-      <c r="B1307" t="inlineStr"/>
+      <c r="B1307" t="n">
+        <v>94</v>
+      </c>
       <c r="C1307" t="n">
         <v>4</v>
       </c>
@@ -16819,7 +16869,9 @@
       <c r="A1308" t="n">
         <v>1307</v>
       </c>
-      <c r="B1308" t="inlineStr"/>
+      <c r="B1308" t="n">
+        <v>94</v>
+      </c>
       <c r="C1308" t="n">
         <v>5</v>
       </c>
@@ -16829,7 +16881,9 @@
       <c r="A1309" t="n">
         <v>1308</v>
       </c>
-      <c r="B1309" t="inlineStr"/>
+      <c r="B1309" t="n">
+        <v>94</v>
+      </c>
       <c r="C1309" t="n">
         <v>6</v>
       </c>
@@ -16839,7 +16893,9 @@
       <c r="A1310" t="n">
         <v>1309</v>
       </c>
-      <c r="B1310" t="inlineStr"/>
+      <c r="B1310" t="n">
+        <v>94</v>
+      </c>
       <c r="C1310" t="n">
         <v>7</v>
       </c>
@@ -16851,7 +16907,9 @@
       <c r="A1311" t="n">
         <v>1310</v>
       </c>
-      <c r="B1311" t="inlineStr"/>
+      <c r="B1311" t="n">
+        <v>94</v>
+      </c>
       <c r="C1311" t="n">
         <v>8</v>
       </c>
@@ -16861,7 +16919,9 @@
       <c r="A1312" t="n">
         <v>1311</v>
       </c>
-      <c r="B1312" t="inlineStr"/>
+      <c r="B1312" t="n">
+        <v>94</v>
+      </c>
       <c r="C1312" t="n">
         <v>9</v>
       </c>
@@ -16871,7 +16931,9 @@
       <c r="A1313" t="n">
         <v>1312</v>
       </c>
-      <c r="B1313" t="inlineStr"/>
+      <c r="B1313" t="n">
+        <v>94</v>
+      </c>
       <c r="C1313" t="n">
         <v>10</v>
       </c>
@@ -16881,7 +16943,9 @@
       <c r="A1314" t="n">
         <v>1313</v>
       </c>
-      <c r="B1314" t="inlineStr"/>
+      <c r="B1314" t="n">
+        <v>94</v>
+      </c>
       <c r="C1314" t="n">
         <v>11</v>
       </c>
@@ -16893,7 +16957,9 @@
       <c r="A1315" t="n">
         <v>1314</v>
       </c>
-      <c r="B1315" t="inlineStr"/>
+      <c r="B1315" t="n">
+        <v>94</v>
+      </c>
       <c r="C1315" t="n">
         <v>12</v>
       </c>
@@ -16903,7 +16969,9 @@
       <c r="A1316" t="n">
         <v>1315</v>
       </c>
-      <c r="B1316" t="inlineStr"/>
+      <c r="B1316" t="n">
+        <v>94</v>
+      </c>
       <c r="C1316" t="n">
         <v>13</v>
       </c>
@@ -16913,7 +16981,9 @@
       <c r="A1317" t="n">
         <v>1316</v>
       </c>
-      <c r="B1317" t="inlineStr"/>
+      <c r="B1317" t="n">
+        <v>94</v>
+      </c>
       <c r="C1317" t="n">
         <v>14</v>
       </c>
@@ -16923,7 +16993,9 @@
       <c r="A1318" t="n">
         <v>1317</v>
       </c>
-      <c r="B1318" t="inlineStr"/>
+      <c r="B1318" t="n">
+        <v>94</v>
+      </c>
       <c r="C1318" t="n">
         <v>15</v>
       </c>
@@ -16935,7 +17007,9 @@
       <c r="A1319" t="n">
         <v>1318</v>
       </c>
-      <c r="B1319" t="inlineStr"/>
+      <c r="B1319" t="n">
+        <v>94</v>
+      </c>
       <c r="C1319" t="n">
         <v>16</v>
       </c>
@@ -16945,7 +17019,9 @@
       <c r="A1320" t="n">
         <v>1319</v>
       </c>
-      <c r="B1320" t="inlineStr"/>
+      <c r="B1320" t="n">
+        <v>94</v>
+      </c>
       <c r="C1320" t="n">
         <v>17</v>
       </c>
@@ -16955,7 +17031,9 @@
       <c r="A1321" t="n">
         <v>1320</v>
       </c>
-      <c r="B1321" t="inlineStr"/>
+      <c r="B1321" t="n">
+        <v>94</v>
+      </c>
       <c r="C1321" t="n">
         <v>18</v>
       </c>
@@ -16965,7 +17043,9 @@
       <c r="A1322" t="n">
         <v>1321</v>
       </c>
-      <c r="B1322" t="inlineStr"/>
+      <c r="B1322" t="n">
+        <v>94</v>
+      </c>
       <c r="C1322" t="n">
         <v>19</v>
       </c>
@@ -16977,7 +17057,9 @@
       <c r="A1323" t="n">
         <v>1322</v>
       </c>
-      <c r="B1323" t="inlineStr"/>
+      <c r="B1323" t="n">
+        <v>94</v>
+      </c>
       <c r="C1323" t="n">
         <v>20</v>
       </c>
@@ -16987,7 +17069,9 @@
       <c r="A1324" t="n">
         <v>1323</v>
       </c>
-      <c r="B1324" t="inlineStr"/>
+      <c r="B1324" t="n">
+        <v>94</v>
+      </c>
       <c r="C1324" t="n">
         <v>21</v>
       </c>
@@ -16997,7 +17081,9 @@
       <c r="A1325" t="n">
         <v>1324</v>
       </c>
-      <c r="B1325" t="inlineStr"/>
+      <c r="B1325" t="n">
+        <v>95</v>
+      </c>
       <c r="C1325" t="n">
         <v>1</v>
       </c>
@@ -17007,7 +17093,9 @@
       <c r="A1326" t="n">
         <v>1325</v>
       </c>
-      <c r="B1326" t="inlineStr"/>
+      <c r="B1326" t="n">
+        <v>95</v>
+      </c>
       <c r="C1326" t="n">
         <v>6</v>
       </c>
@@ -17017,7 +17105,9 @@
       <c r="A1327" t="n">
         <v>1326</v>
       </c>
-      <c r="B1327" t="inlineStr"/>
+      <c r="B1327" t="n">
+        <v>95</v>
+      </c>
       <c r="C1327" t="n">
         <v>3</v>
       </c>
@@ -17027,7 +17117,9 @@
       <c r="A1328" t="n">
         <v>1327</v>
       </c>
-      <c r="B1328" t="inlineStr"/>
+      <c r="B1328" t="n">
+        <v>95</v>
+      </c>
       <c r="C1328" t="n">
         <v>4</v>
       </c>
@@ -17037,7 +17129,9 @@
       <c r="A1329" t="n">
         <v>1328</v>
       </c>
-      <c r="B1329" t="inlineStr"/>
+      <c r="B1329" t="n">
+        <v>95</v>
+      </c>
       <c r="C1329" t="n">
         <v>5</v>
       </c>
@@ -17047,7 +17141,9 @@
       <c r="A1330" t="n">
         <v>1329</v>
       </c>
-      <c r="B1330" t="inlineStr"/>
+      <c r="B1330" t="n">
+        <v>95</v>
+      </c>
       <c r="C1330" t="n">
         <v>6</v>
       </c>
@@ -17057,7 +17153,9 @@
       <c r="A1331" t="n">
         <v>1330</v>
       </c>
-      <c r="B1331" t="inlineStr"/>
+      <c r="B1331" t="n">
+        <v>95</v>
+      </c>
       <c r="C1331" t="n">
         <v>7</v>
       </c>
@@ -17067,7 +17165,9 @@
       <c r="A1332" t="n">
         <v>1331</v>
       </c>
-      <c r="B1332" t="inlineStr"/>
+      <c r="B1332" t="n">
+        <v>95</v>
+      </c>
       <c r="C1332" t="n">
         <v>8</v>
       </c>
@@ -17077,7 +17177,9 @@
       <c r="A1333" t="n">
         <v>1332</v>
       </c>
-      <c r="B1333" t="inlineStr"/>
+      <c r="B1333" t="n">
+        <v>95</v>
+      </c>
       <c r="C1333" t="n">
         <v>9</v>
       </c>
@@ -17087,7 +17189,9 @@
       <c r="A1334" t="n">
         <v>1333</v>
       </c>
-      <c r="B1334" t="inlineStr"/>
+      <c r="B1334" t="n">
+        <v>95</v>
+      </c>
       <c r="C1334" t="n">
         <v>10</v>
       </c>
@@ -17097,7 +17201,9 @@
       <c r="A1335" t="n">
         <v>1334</v>
       </c>
-      <c r="B1335" t="inlineStr"/>
+      <c r="B1335" t="n">
+        <v>95</v>
+      </c>
       <c r="C1335" t="n">
         <v>11</v>
       </c>
@@ -17107,7 +17213,9 @@
       <c r="A1336" t="n">
         <v>1335</v>
       </c>
-      <c r="B1336" t="inlineStr"/>
+      <c r="B1336" t="n">
+        <v>95</v>
+      </c>
       <c r="C1336" t="n">
         <v>12</v>
       </c>
@@ -17117,7 +17225,9 @@
       <c r="A1337" t="n">
         <v>1336</v>
       </c>
-      <c r="B1337" t="inlineStr"/>
+      <c r="B1337" t="n">
+        <v>95</v>
+      </c>
       <c r="C1337" t="n">
         <v>13</v>
       </c>
@@ -17127,7 +17237,9 @@
       <c r="A1338" t="n">
         <v>1337</v>
       </c>
-      <c r="B1338" t="inlineStr"/>
+      <c r="B1338" t="n">
+        <v>95</v>
+      </c>
       <c r="C1338" t="n">
         <v>14</v>
       </c>
@@ -17137,7 +17249,9 @@
       <c r="A1339" t="n">
         <v>1338</v>
       </c>
-      <c r="B1339" t="inlineStr"/>
+      <c r="B1339" t="n">
+        <v>95</v>
+      </c>
       <c r="C1339" t="n">
         <v>15</v>
       </c>
@@ -17147,7 +17261,9 @@
       <c r="A1340" t="n">
         <v>1339</v>
       </c>
-      <c r="B1340" t="inlineStr"/>
+      <c r="B1340" t="n">
+        <v>95</v>
+      </c>
       <c r="C1340" t="n">
         <v>16</v>
       </c>
@@ -17157,7 +17273,9 @@
       <c r="A1341" t="n">
         <v>1340</v>
       </c>
-      <c r="B1341" t="inlineStr"/>
+      <c r="B1341" t="n">
+        <v>95</v>
+      </c>
       <c r="C1341" t="n">
         <v>17</v>
       </c>
@@ -17167,7 +17285,9 @@
       <c r="A1342" t="n">
         <v>1341</v>
       </c>
-      <c r="B1342" t="inlineStr"/>
+      <c r="B1342" t="n">
+        <v>95</v>
+      </c>
       <c r="C1342" t="n">
         <v>18</v>
       </c>
@@ -17177,7 +17297,9 @@
       <c r="A1343" t="n">
         <v>1342</v>
       </c>
-      <c r="B1343" t="inlineStr"/>
+      <c r="B1343" t="n">
+        <v>95</v>
+      </c>
       <c r="C1343" t="n">
         <v>19</v>
       </c>
@@ -17187,7 +17309,9 @@
       <c r="A1344" t="n">
         <v>1343</v>
       </c>
-      <c r="B1344" t="inlineStr"/>
+      <c r="B1344" t="n">
+        <v>95</v>
+      </c>
       <c r="C1344" t="n">
         <v>20</v>
       </c>
@@ -17197,7 +17321,9 @@
       <c r="A1345" t="n">
         <v>1344</v>
       </c>
-      <c r="B1345" t="inlineStr"/>
+      <c r="B1345" t="n">
+        <v>95</v>
+      </c>
       <c r="C1345" t="n">
         <v>21</v>
       </c>
@@ -17207,7 +17333,9 @@
       <c r="A1346" t="n">
         <v>1345</v>
       </c>
-      <c r="B1346" t="inlineStr"/>
+      <c r="B1346" t="n">
+        <v>96</v>
+      </c>
       <c r="C1346" t="n">
         <v>1</v>
       </c>
@@ -17219,7 +17347,9 @@
       <c r="A1347" t="n">
         <v>1346</v>
       </c>
-      <c r="B1347" t="inlineStr"/>
+      <c r="B1347" t="n">
+        <v>96</v>
+      </c>
       <c r="C1347" t="n">
         <v>6</v>
       </c>
@@ -17229,7 +17359,9 @@
       <c r="A1348" t="n">
         <v>1347</v>
       </c>
-      <c r="B1348" t="inlineStr"/>
+      <c r="B1348" t="n">
+        <v>96</v>
+      </c>
       <c r="C1348" t="n">
         <v>3</v>
       </c>
@@ -17241,7 +17373,9 @@
       <c r="A1349" t="n">
         <v>1348</v>
       </c>
-      <c r="B1349" t="inlineStr"/>
+      <c r="B1349" t="n">
+        <v>96</v>
+      </c>
       <c r="C1349" t="n">
         <v>4</v>
       </c>
@@ -17251,7 +17385,9 @@
       <c r="A1350" t="n">
         <v>1349</v>
       </c>
-      <c r="B1350" t="inlineStr"/>
+      <c r="B1350" t="n">
+        <v>96</v>
+      </c>
       <c r="C1350" t="n">
         <v>5</v>
       </c>
@@ -17263,7 +17399,9 @@
       <c r="A1351" t="n">
         <v>1350</v>
       </c>
-      <c r="B1351" t="inlineStr"/>
+      <c r="B1351" t="n">
+        <v>96</v>
+      </c>
       <c r="C1351" t="n">
         <v>6</v>
       </c>
@@ -17273,7 +17411,9 @@
       <c r="A1352" t="n">
         <v>1351</v>
       </c>
-      <c r="B1352" t="inlineStr"/>
+      <c r="B1352" t="n">
+        <v>96</v>
+      </c>
       <c r="C1352" t="n">
         <v>7</v>
       </c>
@@ -17285,7 +17425,9 @@
       <c r="A1353" t="n">
         <v>1352</v>
       </c>
-      <c r="B1353" t="inlineStr"/>
+      <c r="B1353" t="n">
+        <v>96</v>
+      </c>
       <c r="C1353" t="n">
         <v>8</v>
       </c>
@@ -17295,7 +17437,9 @@
       <c r="A1354" t="n">
         <v>1353</v>
       </c>
-      <c r="B1354" t="inlineStr"/>
+      <c r="B1354" t="n">
+        <v>96</v>
+      </c>
       <c r="C1354" t="n">
         <v>9</v>
       </c>
@@ -17307,7 +17451,9 @@
       <c r="A1355" t="n">
         <v>1354</v>
       </c>
-      <c r="B1355" t="inlineStr"/>
+      <c r="B1355" t="n">
+        <v>96</v>
+      </c>
       <c r="C1355" t="n">
         <v>10</v>
       </c>
@@ -17317,7 +17463,9 @@
       <c r="A1356" t="n">
         <v>1355</v>
       </c>
-      <c r="B1356" t="inlineStr"/>
+      <c r="B1356" t="n">
+        <v>96</v>
+      </c>
       <c r="C1356" t="n">
         <v>11</v>
       </c>
@@ -17327,7 +17475,9 @@
       <c r="A1357" t="n">
         <v>1356</v>
       </c>
-      <c r="B1357" t="inlineStr"/>
+      <c r="B1357" t="n">
+        <v>96</v>
+      </c>
       <c r="C1357" t="n">
         <v>12</v>
       </c>
@@ -17337,7 +17487,9 @@
       <c r="A1358" t="n">
         <v>1357</v>
       </c>
-      <c r="B1358" t="inlineStr"/>
+      <c r="B1358" t="n">
+        <v>96</v>
+      </c>
       <c r="C1358" t="n">
         <v>13</v>
       </c>
@@ -17349,7 +17501,9 @@
       <c r="A1359" t="n">
         <v>1358</v>
       </c>
-      <c r="B1359" t="inlineStr"/>
+      <c r="B1359" t="n">
+        <v>96</v>
+      </c>
       <c r="C1359" t="n">
         <v>14</v>
       </c>
@@ -17359,7 +17513,9 @@
       <c r="A1360" t="n">
         <v>1359</v>
       </c>
-      <c r="B1360" t="inlineStr"/>
+      <c r="B1360" t="n">
+        <v>96</v>
+      </c>
       <c r="C1360" t="n">
         <v>15</v>
       </c>
@@ -17371,7 +17527,9 @@
       <c r="A1361" t="n">
         <v>1360</v>
       </c>
-      <c r="B1361" t="inlineStr"/>
+      <c r="B1361" t="n">
+        <v>96</v>
+      </c>
       <c r="C1361" t="n">
         <v>16</v>
       </c>
@@ -17381,7 +17539,9 @@
       <c r="A1362" t="n">
         <v>1361</v>
       </c>
-      <c r="B1362" t="inlineStr"/>
+      <c r="B1362" t="n">
+        <v>96</v>
+      </c>
       <c r="C1362" t="n">
         <v>17</v>
       </c>
@@ -17393,7 +17553,9 @@
       <c r="A1363" t="n">
         <v>1362</v>
       </c>
-      <c r="B1363" t="inlineStr"/>
+      <c r="B1363" t="n">
+        <v>96</v>
+      </c>
       <c r="C1363" t="n">
         <v>18</v>
       </c>
@@ -17403,7 +17565,9 @@
       <c r="A1364" t="n">
         <v>1363</v>
       </c>
-      <c r="B1364" t="inlineStr"/>
+      <c r="B1364" t="n">
+        <v>96</v>
+      </c>
       <c r="C1364" t="n">
         <v>19</v>
       </c>
@@ -17415,7 +17579,9 @@
       <c r="A1365" t="n">
         <v>1364</v>
       </c>
-      <c r="B1365" t="inlineStr"/>
+      <c r="B1365" t="n">
+        <v>96</v>
+      </c>
       <c r="C1365" t="n">
         <v>20</v>
       </c>
@@ -17425,7 +17591,9 @@
       <c r="A1366" t="n">
         <v>1365</v>
       </c>
-      <c r="B1366" t="inlineStr"/>
+      <c r="B1366" t="n">
+        <v>96</v>
+      </c>
       <c r="C1366" t="n">
         <v>21</v>
       </c>
@@ -17437,7 +17605,9 @@
       <c r="A1367" t="n">
         <v>1366</v>
       </c>
-      <c r="B1367" t="inlineStr"/>
+      <c r="B1367" t="n">
+        <v>97</v>
+      </c>
       <c r="C1367" t="n">
         <v>1</v>
       </c>
@@ -17449,7 +17619,9 @@
       <c r="A1368" t="n">
         <v>1367</v>
       </c>
-      <c r="B1368" t="inlineStr"/>
+      <c r="B1368" t="n">
+        <v>97</v>
+      </c>
       <c r="C1368" t="n">
         <v>6</v>
       </c>
@@ -17459,7 +17631,9 @@
       <c r="A1369" t="n">
         <v>1368</v>
       </c>
-      <c r="B1369" t="inlineStr"/>
+      <c r="B1369" t="n">
+        <v>97</v>
+      </c>
       <c r="C1369" t="n">
         <v>3</v>
       </c>
@@ -17471,7 +17645,9 @@
       <c r="A1370" t="n">
         <v>1369</v>
       </c>
-      <c r="B1370" t="inlineStr"/>
+      <c r="B1370" t="n">
+        <v>97</v>
+      </c>
       <c r="C1370" t="n">
         <v>4</v>
       </c>
@@ -17481,7 +17657,9 @@
       <c r="A1371" t="n">
         <v>1370</v>
       </c>
-      <c r="B1371" t="inlineStr"/>
+      <c r="B1371" t="n">
+        <v>97</v>
+      </c>
       <c r="C1371" t="n">
         <v>5</v>
       </c>
@@ -17493,7 +17671,9 @@
       <c r="A1372" t="n">
         <v>1371</v>
       </c>
-      <c r="B1372" t="inlineStr"/>
+      <c r="B1372" t="n">
+        <v>97</v>
+      </c>
       <c r="C1372" t="n">
         <v>6</v>
       </c>
@@ -17505,7 +17685,9 @@
       <c r="A1373" t="n">
         <v>1372</v>
       </c>
-      <c r="B1373" t="inlineStr"/>
+      <c r="B1373" t="n">
+        <v>97</v>
+      </c>
       <c r="C1373" t="n">
         <v>7</v>
       </c>
@@ -17517,7 +17699,9 @@
       <c r="A1374" t="n">
         <v>1373</v>
       </c>
-      <c r="B1374" t="inlineStr"/>
+      <c r="B1374" t="n">
+        <v>97</v>
+      </c>
       <c r="C1374" t="n">
         <v>8</v>
       </c>
@@ -17529,7 +17713,9 @@
       <c r="A1375" t="n">
         <v>1374</v>
       </c>
-      <c r="B1375" t="inlineStr"/>
+      <c r="B1375" t="n">
+        <v>97</v>
+      </c>
       <c r="C1375" t="n">
         <v>9</v>
       </c>
@@ -17541,7 +17727,9 @@
       <c r="A1376" t="n">
         <v>1375</v>
       </c>
-      <c r="B1376" t="inlineStr"/>
+      <c r="B1376" t="n">
+        <v>97</v>
+      </c>
       <c r="C1376" t="n">
         <v>10</v>
       </c>
@@ -17551,7 +17739,9 @@
       <c r="A1377" t="n">
         <v>1376</v>
       </c>
-      <c r="B1377" t="inlineStr"/>
+      <c r="B1377" t="n">
+        <v>97</v>
+      </c>
       <c r="C1377" t="n">
         <v>11</v>
       </c>
@@ -17563,7 +17753,9 @@
       <c r="A1378" t="n">
         <v>1377</v>
       </c>
-      <c r="B1378" t="inlineStr"/>
+      <c r="B1378" t="n">
+        <v>97</v>
+      </c>
       <c r="C1378" t="n">
         <v>12</v>
       </c>
@@ -17575,7 +17767,9 @@
       <c r="A1379" t="n">
         <v>1378</v>
       </c>
-      <c r="B1379" t="inlineStr"/>
+      <c r="B1379" t="n">
+        <v>97</v>
+      </c>
       <c r="C1379" t="n">
         <v>13</v>
       </c>
@@ -17587,7 +17781,9 @@
       <c r="A1380" t="n">
         <v>1379</v>
       </c>
-      <c r="B1380" t="inlineStr"/>
+      <c r="B1380" t="n">
+        <v>97</v>
+      </c>
       <c r="C1380" t="n">
         <v>14</v>
       </c>
@@ -17597,7 +17793,9 @@
       <c r="A1381" t="n">
         <v>1380</v>
       </c>
-      <c r="B1381" t="inlineStr"/>
+      <c r="B1381" t="n">
+        <v>97</v>
+      </c>
       <c r="C1381" t="n">
         <v>15</v>
       </c>
@@ -17609,7 +17807,9 @@
       <c r="A1382" t="n">
         <v>1381</v>
       </c>
-      <c r="B1382" t="inlineStr"/>
+      <c r="B1382" t="n">
+        <v>97</v>
+      </c>
       <c r="C1382" t="n">
         <v>16</v>
       </c>
@@ -17621,7 +17821,9 @@
       <c r="A1383" t="n">
         <v>1382</v>
       </c>
-      <c r="B1383" t="inlineStr"/>
+      <c r="B1383" t="n">
+        <v>97</v>
+      </c>
       <c r="C1383" t="n">
         <v>17</v>
       </c>
@@ -17633,7 +17835,9 @@
       <c r="A1384" t="n">
         <v>1383</v>
       </c>
-      <c r="B1384" t="inlineStr"/>
+      <c r="B1384" t="n">
+        <v>97</v>
+      </c>
       <c r="C1384" t="n">
         <v>18</v>
       </c>
@@ -17643,7 +17847,9 @@
       <c r="A1385" t="n">
         <v>1384</v>
       </c>
-      <c r="B1385" t="inlineStr"/>
+      <c r="B1385" t="n">
+        <v>97</v>
+      </c>
       <c r="C1385" t="n">
         <v>19</v>
       </c>
@@ -17655,7 +17861,9 @@
       <c r="A1386" t="n">
         <v>1385</v>
       </c>
-      <c r="B1386" t="inlineStr"/>
+      <c r="B1386" t="n">
+        <v>97</v>
+      </c>
       <c r="C1386" t="n">
         <v>20</v>
       </c>
@@ -17667,7 +17875,9 @@
       <c r="A1387" t="n">
         <v>1386</v>
       </c>
-      <c r="B1387" t="inlineStr"/>
+      <c r="B1387" t="n">
+        <v>97</v>
+      </c>
       <c r="C1387" t="n">
         <v>21</v>
       </c>

</xml_diff>